<commit_message>
feat: update file paths and add template upload explanation text
</commit_message>
<xml_diff>
--- a/Monthly RoA Total - Correct.xlsx
+++ b/Monthly RoA Total - Correct.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bwilzbach\CascadeProjects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\BW Code\CashDragProject\portfolio_optimizer_streamlit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F592E2C-1B79-4BC9-99E3-1841EEAC8E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7E089F4-916D-4652-9AC8-AB01C1A6F1A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8010" yWindow="13155" windowWidth="27015" windowHeight="13095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -553,14 +553,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y19"/>
+  <dimension ref="A1:Y20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.42578125" customWidth="1"/>
     <col min="24" max="24" width="12.7109375" customWidth="1"/>
     <col min="25" max="25" width="14.5703125" customWidth="1"/>
@@ -1681,6 +1682,69 @@
       <c r="X19" s="5"/>
       <c r="Y19" s="5"/>
     </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>45778</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2">
+        <v>4.60156707996138E-2</v>
+      </c>
+      <c r="D20" s="2">
+        <v>9.5751663312759194E-3</v>
+      </c>
+      <c r="E20" s="2">
+        <v>2.9482081213155699E-3</v>
+      </c>
+      <c r="F20" s="2">
+        <v>3.61638486420309E-3</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1.19677490460344E-2</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2">
+        <v>7.8607950851264805E-2</v>
+      </c>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2">
+        <v>6.6286199885192604E-2</v>
+      </c>
+      <c r="L20" s="2">
+        <v>2.13044883464408E-2</v>
+      </c>
+      <c r="M20" s="2">
+        <v>7.56208581480451E-3</v>
+      </c>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2">
+        <v>6.7578221871267795E-4</v>
+      </c>
+      <c r="P20" s="2">
+        <v>4.8534157866455601E-3</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>8.6748451024642494E-3</v>
+      </c>
+      <c r="R20" s="2">
+        <v>-6.7549627172674306E-2</v>
+      </c>
+      <c r="S20" s="2">
+        <v>1.9812116106194998E-2</v>
+      </c>
+      <c r="T20" s="2">
+        <v>1.0157619985705101E-2</v>
+      </c>
+      <c r="U20" s="2">
+        <v>1.65367513349453E-2</v>
+      </c>
+      <c r="V20" s="2">
+        <v>1.4408686922871001E-2</v>
+      </c>
+      <c r="W20" s="2"/>
+      <c r="X20" s="2"/>
+      <c r="Y20" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Excel spreadsheets with latest data changes
</commit_message>
<xml_diff>
--- a/Monthly RoA Total - Correct.xlsx
+++ b/Monthly RoA Total - Correct.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\BW Code\CashDragProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F3F80F3-C077-4A61-B5BB-05CF7FB97D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7BEB682-80EC-44C3-9916-56527B8DFB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24990" yWindow="6030" windowWidth="27015" windowHeight="13095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30390" yWindow="6660" windowWidth="25560" windowHeight="17490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Month</t>
   </si>
@@ -162,6 +162,15 @@
   </si>
   <si>
     <t>SHORT TERM F1</t>
+  </si>
+  <si>
+    <t>CLO AAA ETF F1</t>
+  </si>
+  <si>
+    <t>CLO MEZZ F1</t>
+  </si>
+  <si>
+    <t>TRUPS MEZZ F1</t>
   </si>
 </sst>
 </file>
@@ -209,7 +218,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -232,12 +241,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -248,6 +268,10 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -553,7 +577,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y20"/>
+  <dimension ref="A1:AB21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
@@ -562,12 +586,19 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.42578125" customWidth="1"/>
     <col min="24" max="24" width="12.7109375" customWidth="1"/>
     <col min="25" max="25" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -643,8 +674,17 @@
       <c r="Y1" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="Z1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB1" s="7" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
@@ -689,7 +729,7 @@
       <c r="X2" s="5"/>
       <c r="Y2" s="5"/>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
@@ -734,7 +774,7 @@
       <c r="X3" s="5"/>
       <c r="Y3" s="5"/>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>24</v>
       </c>
@@ -785,7 +825,7 @@
       <c r="X4" s="5"/>
       <c r="Y4" s="5"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
@@ -836,7 +876,7 @@
       <c r="X5" s="5"/>
       <c r="Y5" s="5"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>26</v>
       </c>
@@ -887,7 +927,7 @@
       <c r="X6" s="5"/>
       <c r="Y6" s="5"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>27</v>
       </c>
@@ -938,7 +978,7 @@
       <c r="X7" s="5"/>
       <c r="Y7" s="5"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
@@ -993,7 +1033,7 @@
       </c>
       <c r="Y8" s="5"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>29</v>
       </c>
@@ -1050,7 +1090,7 @@
       </c>
       <c r="Y9" s="5"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>30</v>
       </c>
@@ -1115,7 +1155,7 @@
         <v>2.380923794495916E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>31</v>
       </c>
@@ -1182,7 +1222,7 @@
         <v>2.358809691728117E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>32</v>
       </c>
@@ -1243,7 +1283,7 @@
       <c r="X12" s="5"/>
       <c r="Y12" s="5"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>33</v>
       </c>
@@ -1304,7 +1344,7 @@
       <c r="X13" s="5"/>
       <c r="Y13" s="5"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>34</v>
       </c>
@@ -1363,7 +1403,7 @@
       <c r="X14" s="5"/>
       <c r="Y14" s="5"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>35</v>
       </c>
@@ -1422,7 +1462,7 @@
       <c r="X15" s="5"/>
       <c r="Y15" s="5"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>36</v>
       </c>
@@ -1489,7 +1529,7 @@
       <c r="X16" s="5"/>
       <c r="Y16" s="5"/>
     </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>37</v>
       </c>
@@ -1556,7 +1596,7 @@
       <c r="X17" s="5"/>
       <c r="Y17" s="5"/>
     </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>38</v>
       </c>
@@ -1619,7 +1659,7 @@
       <c r="X18" s="5"/>
       <c r="Y18" s="5"/>
     </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>39</v>
       </c>
@@ -1682,7 +1722,7 @@
       <c r="X19" s="5"/>
       <c r="Y19" s="5"/>
     </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>45778</v>
       </c>
@@ -1744,6 +1784,59 @@
       <c r="W20" s="2"/>
       <c r="X20" s="2"/>
       <c r="Y20" s="2"/>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>45809</v>
+      </c>
+      <c r="C21" s="6">
+        <v>2.24E-2</v>
+      </c>
+      <c r="D21" s="6">
+        <v>3.5900000000000001E-2</v>
+      </c>
+      <c r="E21" s="6">
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="F21" s="6">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K21" s="2">
+        <v>4.9824343700000003E-2</v>
+      </c>
+      <c r="L21" s="2">
+        <v>1.1138162199999999E-2</v>
+      </c>
+      <c r="M21" s="2">
+        <v>6.1878486000000003E-3</v>
+      </c>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2">
+        <v>1.17919488E-2</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>3.9378215899999999E-2</v>
+      </c>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2">
+        <v>5.6501178399999998E-2</v>
+      </c>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="2"/>
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="2">
+        <v>3.2513108000000002E-3</v>
+      </c>
+      <c r="AA21" s="2">
+        <v>9.0110095000000001E-3</v>
+      </c>
+      <c r="AB21" s="2">
+        <v>9.0373437000000004E-3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1752,6 +1845,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100572F39F379485941A052184567561C33" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c3822a37d5a98658884236550ca66e7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="62537be5-96bf-45a7-b525-5d0c59b29924" xmlns:ns4="b4b63fd0-8e4c-468f-bbaf-f55c8da78e53" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fe85f39d6345a37fe79994e516824198" ns3:_="" ns4:_="">
     <xsd:import namespace="62537be5-96bf-45a7-b525-5d0c59b29924"/>
@@ -1954,15 +2056,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1972,6 +2065,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2CBFB7D-2BFD-4688-A356-0D1DE0FBEE38}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2FF66538-16F2-4126-92B0-052E532F25D4}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1986,14 +2087,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2CBFB7D-2BFD-4688-A356-0D1DE0FBEE38}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>